<commit_message>
Added Excel Function in calc.xlsx
</commit_message>
<xml_diff>
--- a/Prototype/PHPSCRIPTS/JASON/calc.xlsx
+++ b/Prototype/PHPSCRIPTS/JASON/calc.xlsx
@@ -25,6 +25,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -54,8 +57,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,7 +377,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,6 +386,7 @@
       <c r="A1">
         <v>3</v>
       </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -438,5 +443,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>